<commit_message>
Added Temp Documentation files
Added setup and coverage report for sprint 0
Added temp diagrams in document directory
</commit_message>
<xml_diff>
--- a/sprint/sprint_1/Sprint 1 backlog.xlsx
+++ b/sprint/sprint_1/Sprint 1 backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jg00242\Documents\dev\UWG-Capstone-Group1\sprint\sprint_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C61E55FE-CE8A-4BCF-ABAD-711594384438}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D05C0E-33B4-4451-AE3B-42DBA963FFE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="26116" windowHeight="13335" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2205" yWindow="2205" windowWidth="19440" windowHeight="9578" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Related User Story</t>
   </si>
@@ -123,9 +123,6 @@
   </si>
   <si>
     <t>User ability to use credentials to login</t>
-  </si>
-  <si>
-    <t>s</t>
   </si>
 </sst>
 </file>
@@ -750,8 +747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G1006"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -1009,9 +1006,7 @@
     </row>
     <row r="22" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A22" s="2"/>
-      <c r="B22" s="2" t="s">
-        <v>30</v>
-      </c>
+      <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>

</xml_diff>